<commit_message>
all words in one file
</commit_message>
<xml_diff>
--- a/exp_words.xlsx
+++ b/exp_words.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="984" yWindow="0" windowWidth="16296" windowHeight="7812" activeTab="1"/>
+    <workbookView xWindow="1968" yWindow="0" windowWidth="16296" windowHeight="7812" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ז2-ז3" sheetId="1" r:id="rId1"/>
+    <sheet name="Adaptation" sheetId="2" r:id="rId2"/>
+    <sheet name="localizer" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="649">
   <si>
     <t>גחזל</t>
   </si>
@@ -753,9 +754,6 @@
     <t>ד</t>
   </si>
   <si>
-    <t>ז</t>
-  </si>
-  <si>
     <t>ח</t>
   </si>
   <si>
@@ -798,12 +796,6 @@
     <t>ת</t>
   </si>
   <si>
-    <t>ף</t>
-  </si>
-  <si>
-    <t>ץ</t>
-  </si>
-  <si>
     <t>תגנבו</t>
   </si>
   <si>
@@ -1003,19 +995,1008 @@
   </si>
   <si>
     <t>חקרנו</t>
+  </si>
+  <si>
+    <t>קערה</t>
+  </si>
+  <si>
+    <t>זמרת</t>
+  </si>
+  <si>
+    <t>פשרה</t>
+  </si>
+  <si>
+    <t>מחבר</t>
+  </si>
+  <si>
+    <t>מכסה</t>
+  </si>
+  <si>
+    <t>חשבה</t>
+  </si>
+  <si>
+    <t>קפצת</t>
+  </si>
+  <si>
+    <t>לסרק</t>
+  </si>
+  <si>
+    <t>מדען</t>
+  </si>
+  <si>
+    <t>דגרה</t>
+  </si>
+  <si>
+    <t>לאתר</t>
+  </si>
+  <si>
+    <t>התקלח</t>
+  </si>
+  <si>
+    <t>התגבר</t>
+  </si>
+  <si>
+    <t>תברחי</t>
+  </si>
+  <si>
+    <t>מבשרת</t>
+  </si>
+  <si>
+    <t>תוספת</t>
+  </si>
+  <si>
+    <t>קרעה</t>
+  </si>
+  <si>
+    <t>זרמת</t>
+  </si>
+  <si>
+    <t>פרשה</t>
+  </si>
+  <si>
+    <t>מבחר</t>
+  </si>
+  <si>
+    <t>מסכה</t>
+  </si>
+  <si>
+    <t>חבשה</t>
+  </si>
+  <si>
+    <t>קצפת</t>
+  </si>
+  <si>
+    <t>לרסק</t>
+  </si>
+  <si>
+    <t>מעדן</t>
+  </si>
+  <si>
+    <t>דרגה</t>
+  </si>
+  <si>
+    <t>לתאר</t>
+  </si>
+  <si>
+    <t>התלקח</t>
+  </si>
+  <si>
+    <t>התבגר</t>
+  </si>
+  <si>
+    <t>תבחרי</t>
+  </si>
+  <si>
+    <t>מברשת</t>
+  </si>
+  <si>
+    <t>תופסת</t>
+  </si>
+  <si>
+    <t>מקריב</t>
+  </si>
+  <si>
+    <t>מרקיב</t>
+  </si>
+  <si>
+    <t>לבחוש</t>
+  </si>
+  <si>
+    <t>לחבוש</t>
+  </si>
+  <si>
+    <t>יבדקו</t>
+  </si>
+  <si>
+    <t>ידבקו</t>
+  </si>
+  <si>
+    <t>ישפוט</t>
+  </si>
+  <si>
+    <t>יפשוט</t>
+  </si>
+  <si>
+    <t>מרגיל</t>
+  </si>
+  <si>
+    <t>מגריל</t>
+  </si>
+  <si>
+    <t>יתארו</t>
+  </si>
+  <si>
+    <t>יאתרו</t>
+  </si>
+  <si>
+    <t>להכשיר</t>
+  </si>
+  <si>
+    <t>להשכיר</t>
+  </si>
+  <si>
+    <t>יחרקו</t>
+  </si>
+  <si>
+    <t>יחקרו</t>
+  </si>
+  <si>
+    <t>חושבת</t>
+  </si>
+  <si>
+    <t>חובשת</t>
+  </si>
+  <si>
+    <t>פורשת</t>
+  </si>
+  <si>
+    <t>פושרת</t>
+  </si>
+  <si>
+    <t>תשקרו</t>
+  </si>
+  <si>
+    <t>תשרקו</t>
+  </si>
+  <si>
+    <t>לעמוד</t>
+  </si>
+  <si>
+    <t>למעוד</t>
+  </si>
+  <si>
+    <t>יגרעו</t>
+  </si>
+  <si>
+    <t>ירגעו</t>
+  </si>
+  <si>
+    <t>מפרות</t>
+  </si>
+  <si>
+    <t>מרפות</t>
+  </si>
+  <si>
+    <t>לצבוע</t>
+  </si>
+  <si>
+    <t>פיטרה</t>
+  </si>
+  <si>
+    <t>פירטה</t>
+  </si>
+  <si>
+    <t>בקרים</t>
+  </si>
+  <si>
+    <t>ברקים</t>
+  </si>
+  <si>
+    <t>ברחה</t>
+  </si>
+  <si>
+    <t>בחרה</t>
+  </si>
+  <si>
+    <t>חוקרת</t>
+  </si>
+  <si>
+    <t>חורקת</t>
+  </si>
+  <si>
+    <t>חודשים</t>
+  </si>
+  <si>
+    <t>חושדים</t>
+  </si>
+  <si>
+    <t>יקשרו</t>
+  </si>
+  <si>
+    <t>ישקרו</t>
+  </si>
+  <si>
+    <t>חרבות</t>
+  </si>
+  <si>
+    <t>חברות</t>
+  </si>
+  <si>
+    <t>ערבית</t>
+  </si>
+  <si>
+    <t>עברית</t>
+  </si>
+  <si>
+    <t>מדענים</t>
+  </si>
+  <si>
+    <t>מעדנים</t>
+  </si>
+  <si>
+    <t>נופשים</t>
+  </si>
+  <si>
+    <t>נושפים</t>
+  </si>
+  <si>
+    <t>קוצרים</t>
+  </si>
+  <si>
+    <t>קורצים</t>
+  </si>
+  <si>
+    <t>גלמים</t>
+  </si>
+  <si>
+    <t>גמלים</t>
+  </si>
+  <si>
+    <t>קלפים</t>
+  </si>
+  <si>
+    <t>קפלים</t>
+  </si>
+  <si>
+    <t>הפסיק</t>
+  </si>
+  <si>
+    <t>הספיק</t>
+  </si>
+  <si>
+    <t>מקשר</t>
+  </si>
+  <si>
+    <t>משקר</t>
+  </si>
+  <si>
+    <t>רשעים</t>
+  </si>
+  <si>
+    <t>רעשים</t>
+  </si>
+  <si>
+    <t>כבאים</t>
+  </si>
+  <si>
+    <t>כאבים</t>
+  </si>
+  <si>
+    <t>תאנים</t>
+  </si>
+  <si>
+    <t>תנאים</t>
+  </si>
+  <si>
+    <t>מפסידה</t>
+  </si>
+  <si>
+    <t>מספידה</t>
+  </si>
+  <si>
+    <t>חוברות</t>
+  </si>
+  <si>
+    <t>חורבות</t>
+  </si>
+  <si>
+    <t>חוזרים</t>
+  </si>
+  <si>
+    <t>חורזים</t>
+  </si>
+  <si>
+    <t>תלחשו</t>
+  </si>
+  <si>
+    <t>תחלשו</t>
+  </si>
+  <si>
+    <t>מתגרשים</t>
+  </si>
+  <si>
+    <t>מתרגשים</t>
+  </si>
+  <si>
+    <t xml:space="preserve">תמחקו </t>
+  </si>
+  <si>
+    <t>תחמקו</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ירצחו </t>
+  </si>
+  <si>
+    <t>יצרחו</t>
+  </si>
+  <si>
+    <t xml:space="preserve">לעמוד </t>
+  </si>
+  <si>
+    <t>יצרפו</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ירצפו </t>
+  </si>
+  <si>
+    <t xml:space="preserve">תסרקי    </t>
+  </si>
+  <si>
+    <t>תסקרי</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מדרגה </t>
+  </si>
+  <si>
+    <t>מדגרה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">חבלן   </t>
+  </si>
+  <si>
+    <t>חלבן</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> הרעשנו</t>
+  </si>
+  <si>
+    <t>הרשענו</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> סוגרת</t>
+  </si>
+  <si>
+    <t>סורגת</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> חשדן</t>
+  </si>
+  <si>
+    <t>חדשן</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> נדבק</t>
+  </si>
+  <si>
+    <t>נבדק</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ילחש </t>
+  </si>
+  <si>
+    <t>יחלש</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> לעמול</t>
+  </si>
+  <si>
+    <t>למעול</t>
+  </si>
+  <si>
+    <t xml:space="preserve">פרשנות </t>
+  </si>
+  <si>
+    <t>פשרנות</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מתערבת </t>
+  </si>
+  <si>
+    <t>מתעברת</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  חוקרים</t>
+  </si>
+  <si>
+    <t>חורקים</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ינצח </t>
+  </si>
+  <si>
+    <t>יצנח</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> התנגב</t>
+  </si>
+  <si>
+    <t>התגנב</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> יחבלו</t>
+  </si>
+  <si>
+    <t>יחלבו</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> לקשר</t>
+  </si>
+  <si>
+    <t>לשקר</t>
+  </si>
+  <si>
+    <t>ችኅስር</t>
+  </si>
+  <si>
+    <t>בסדר</t>
+  </si>
+  <si>
+    <t>128762)</t>
+  </si>
+  <si>
+    <t>גינופיט</t>
+  </si>
+  <si>
+    <t>ሩኡምቭ</t>
+  </si>
+  <si>
+    <t>רוצה</t>
+  </si>
+  <si>
+    <t>109110)</t>
+  </si>
+  <si>
+    <t>נולר</t>
+  </si>
+  <si>
+    <t>ትብጅቡኡ</t>
+  </si>
+  <si>
+    <t>אנחנו</t>
+  </si>
+  <si>
+    <t>94163)</t>
+  </si>
+  <si>
+    <t>שוצי</t>
+  </si>
+  <si>
+    <t>ቱኡ፣ል</t>
+  </si>
+  <si>
+    <t>אותך</t>
+  </si>
+  <si>
+    <t>89234)</t>
+  </si>
+  <si>
+    <t>בוף</t>
+  </si>
+  <si>
+    <t>ሁኡስግ</t>
+  </si>
+  <si>
+    <t>יודע</t>
+  </si>
+  <si>
+    <t>89141)</t>
+  </si>
+  <si>
+    <t>חיוולת</t>
+  </si>
+  <si>
+    <t>ቱኡ፣ኡ</t>
+  </si>
+  <si>
+    <t>אותו</t>
+  </si>
+  <si>
+    <t>81989)</t>
+  </si>
+  <si>
+    <t>גומיל</t>
+  </si>
+  <si>
+    <t>ህጉኡክ</t>
+  </si>
+  <si>
+    <t>יכול</t>
+  </si>
+  <si>
+    <t>78217)</t>
+  </si>
+  <si>
+    <t>עוזמת</t>
+  </si>
+  <si>
+    <t>ቱኡ፣ህ</t>
+  </si>
+  <si>
+    <t>אותי</t>
+  </si>
+  <si>
+    <t>73817)</t>
+  </si>
+  <si>
+    <t>מוזף</t>
+  </si>
+  <si>
+    <t>ሁኡ፣ር</t>
+  </si>
+  <si>
+    <t>יותר</t>
+  </si>
+  <si>
+    <t>73799)</t>
+  </si>
+  <si>
+    <t>סנמר</t>
+  </si>
+  <si>
+    <t>ግፏኣሁኡ</t>
+  </si>
+  <si>
+    <t>עכשיו</t>
+  </si>
+  <si>
+    <t>62548)</t>
+  </si>
+  <si>
+    <t>ארפץ</t>
+  </si>
+  <si>
+    <t>ኗኣቩኡ</t>
+  </si>
+  <si>
+    <t>משהו</t>
+  </si>
+  <si>
+    <t>61326)</t>
+  </si>
+  <si>
+    <t>סיצו</t>
+  </si>
+  <si>
+    <t>ክቭሁኡ፣</t>
+  </si>
+  <si>
+    <t>להיות</t>
+  </si>
+  <si>
+    <t>58268)</t>
+  </si>
+  <si>
+    <t>משקז</t>
+  </si>
+  <si>
+    <t>፣ኡስቭ</t>
+  </si>
+  <si>
+    <t>תודה</t>
+  </si>
+  <si>
+    <t>56736)</t>
+  </si>
+  <si>
+    <t>צחתו</t>
+  </si>
+  <si>
+    <t>ብፉኡኢ</t>
+  </si>
+  <si>
+    <t>נכון</t>
+  </si>
+  <si>
+    <t>52845)</t>
+  </si>
+  <si>
+    <t>שרופל</t>
+  </si>
+  <si>
+    <t>ምርህል</t>
+  </si>
+  <si>
+    <t>צריך</t>
+  </si>
+  <si>
+    <t>49621)</t>
+  </si>
+  <si>
+    <t>טקק</t>
+  </si>
+  <si>
+    <t>ክዏኣኡ፣</t>
+  </si>
+  <si>
+    <t>לעשות</t>
+  </si>
+  <si>
+    <t>49337)</t>
+  </si>
+  <si>
+    <t>בולך</t>
+  </si>
+  <si>
+    <t>አሽህንቭ</t>
+  </si>
+  <si>
+    <t>קדימה</t>
+  </si>
+  <si>
+    <t>47464)</t>
+  </si>
+  <si>
+    <t>ישמג</t>
+  </si>
+  <si>
+    <t>ጁኡኣች</t>
+  </si>
+  <si>
+    <t>חושב</t>
+  </si>
+  <si>
+    <t>45687)</t>
+  </si>
+  <si>
+    <t>לומיטר</t>
+  </si>
+  <si>
+    <t>ሁኡስግ፣</t>
+  </si>
+  <si>
+    <t>יודעת</t>
+  </si>
+  <si>
+    <t>42211)</t>
+  </si>
+  <si>
+    <t>עוקה</t>
+  </si>
+  <si>
+    <t>ችትን፣</t>
+  </si>
+  <si>
+    <t>באמת</t>
+  </si>
+  <si>
+    <t>40641)</t>
+  </si>
+  <si>
+    <t>לורג</t>
+  </si>
+  <si>
+    <t>ቭሕሕ፣ሕ</t>
+  </si>
+  <si>
+    <t>הייתי</t>
+  </si>
+  <si>
+    <t>40545)</t>
+  </si>
+  <si>
+    <t>זוגר</t>
+  </si>
+  <si>
+    <t>ጉኡኣቭ</t>
+  </si>
+  <si>
+    <t>עושה</t>
+  </si>
+  <si>
+    <t>37350)</t>
+  </si>
+  <si>
+    <t>אבליעם</t>
+  </si>
+  <si>
+    <t>ችቼአኣቭ</t>
+  </si>
+  <si>
+    <t>בבקשה</t>
+  </si>
+  <si>
+    <t>37312)</t>
+  </si>
+  <si>
+    <t>כוגדת</t>
+  </si>
+  <si>
+    <t>ፗኣኡይ</t>
+  </si>
+  <si>
+    <t>פשוט</t>
+  </si>
+  <si>
+    <t>37158)</t>
+  </si>
+  <si>
+    <t>מתקבש</t>
+  </si>
+  <si>
+    <t>ንቱኡስ</t>
+  </si>
+  <si>
+    <t>מאוד</t>
+  </si>
+  <si>
+    <t>35920)</t>
+  </si>
+  <si>
+    <t>מחוגס</t>
+  </si>
+  <si>
+    <t>ክግዝግዝክ</t>
+  </si>
+  <si>
+    <t>לעזאזל</t>
+  </si>
+  <si>
+    <t>33985)</t>
+  </si>
+  <si>
+    <t>לצובן</t>
+  </si>
+  <si>
+    <t>ብርትቭ</t>
+  </si>
+  <si>
+    <t>נראה</t>
+  </si>
+  <si>
+    <t>33705)</t>
+  </si>
+  <si>
+    <t>נובש</t>
+  </si>
+  <si>
+    <t>ትኩኡቭሆኦ</t>
+  </si>
+  <si>
+    <t>אלוהים</t>
+  </si>
+  <si>
+    <t>33001)</t>
+  </si>
+  <si>
+    <t>צחמר</t>
+  </si>
+  <si>
+    <t>ቭርችቭ</t>
+  </si>
+  <si>
+    <t>הרבה</t>
+  </si>
+  <si>
+    <t>30481)</t>
+  </si>
+  <si>
+    <t>פואש</t>
+  </si>
+  <si>
+    <t>ህፉኡክቭ</t>
+  </si>
+  <si>
+    <t>יכולה</t>
+  </si>
+  <si>
+    <t>29482)</t>
+  </si>
+  <si>
+    <t>קוגם</t>
+  </si>
+  <si>
+    <t>ቱኡንር</t>
+  </si>
+  <si>
+    <t>אומר</t>
+  </si>
+  <si>
+    <t>28861)</t>
+  </si>
+  <si>
+    <t>פצנש</t>
+  </si>
+  <si>
+    <t>ቱኡ፣ኦ</t>
+  </si>
+  <si>
+    <t>אותם</t>
+  </si>
+  <si>
+    <t>28641)</t>
+  </si>
+  <si>
+    <t>עוגץ</t>
+  </si>
+  <si>
+    <t>ክፕብህ</t>
+  </si>
+  <si>
+    <t>לפני</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28409) </t>
+  </si>
+  <si>
+    <t>עיבלו</t>
+  </si>
+  <si>
+    <t>ቩኡክል</t>
+  </si>
+  <si>
+    <t>הולך</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26746) </t>
+  </si>
+  <si>
+    <t>מודיב</t>
+  </si>
+  <si>
+    <t>ክርቱኡ፣</t>
+  </si>
+  <si>
+    <t>לראות</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25601) </t>
+  </si>
+  <si>
+    <t>חסיטל</t>
+  </si>
+  <si>
+    <t>ንዏኣቩኡ</t>
+  </si>
+  <si>
+    <t>מישהו</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25239) </t>
+  </si>
+  <si>
+    <t>גילב</t>
+  </si>
+  <si>
+    <t>ግሽሕሒኢ</t>
+  </si>
+  <si>
+    <t>עדיין</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24791) </t>
+  </si>
+  <si>
+    <t>ችሽሁኡአ</t>
+  </si>
+  <si>
+    <t>בדיוק</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23806) </t>
+  </si>
+  <si>
+    <t>ትቧኣሆኦ</t>
+  </si>
+  <si>
+    <t>אנשים</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22586) </t>
+  </si>
+  <si>
+    <t>ንምይግር</t>
+  </si>
+  <si>
+    <t>מצטער</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22581) </t>
+  </si>
+  <si>
+    <t>ኣኩኡኦ</t>
+  </si>
+  <si>
+    <t>שלום</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21946) </t>
+  </si>
+  <si>
+    <t>ቱኡቭች</t>
+  </si>
+  <si>
+    <t>אוהב</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21477) </t>
+  </si>
+  <si>
+    <t>ጇኣች፣ህ</t>
+  </si>
+  <si>
+    <t>חשבתי</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21032) </t>
+  </si>
+  <si>
+    <t>ክስችር</t>
+  </si>
+  <si>
+    <t>לדבר</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20766) </t>
+  </si>
+  <si>
+    <t>ጁኡኣች፣</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20311) </t>
+  </si>
+  <si>
+    <t>ምርህፍቭ</t>
+  </si>
+  <si>
+    <t>צריכה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20278) </t>
+  </si>
+  <si>
+    <t>፣ንህስ</t>
+  </si>
+  <si>
+    <t>תמיד</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20251) </t>
+  </si>
+  <si>
+    <t>RW</t>
+  </si>
+  <si>
+    <t>PW</t>
+  </si>
+  <si>
+    <t>false-font</t>
+  </si>
+  <si>
+    <t>word-count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0B0080"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1035,14 +2016,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 23" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1323,8 +2313,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N120"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102:B102"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1340,21 +2330,21 @@
         <v>239</v>
       </c>
       <c r="H1">
-        <f>COUNTIF($A:$A,"*" &amp; G1&amp;"*")</f>
+        <f t="shared" ref="H1:H17" si="0">COUNTIF($A:$A,"*" &amp; G1&amp;"*")</f>
         <v>21</v>
       </c>
       <c r="J1" t="s">
         <v>239</v>
       </c>
       <c r="K1">
-        <f>COUNTIF($A:$A,J1&amp;"*")</f>
+        <f t="shared" ref="K1:K17" si="1">COUNTIF($A:$A,J1&amp;"*")</f>
         <v>0</v>
       </c>
       <c r="M1" t="s">
         <v>239</v>
       </c>
       <c r="N1">
-        <f>COUNTIF($A:$A,"*" &amp;M1)</f>
+        <f t="shared" ref="N1:N17" si="2">COUNTIF($A:$A,"*" &amp;M1)</f>
         <v>15</v>
       </c>
     </row>
@@ -1373,21 +2363,21 @@
         <v>240</v>
       </c>
       <c r="H2">
-        <f>COUNTIF($A:$A,"*" &amp; G2&amp;"*")</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="J2" t="s">
         <v>240</v>
       </c>
       <c r="K2">
-        <f>COUNTIF($A:$A,J2&amp;"*")</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="M2" t="s">
         <v>240</v>
       </c>
       <c r="N2">
-        <f>COUNTIF($A:$A,"*" &amp;M2)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
@@ -1402,21 +2392,21 @@
         <v>241</v>
       </c>
       <c r="H3">
-        <f>COUNTIF($A:$A,"*" &amp; G3&amp;"*")</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="J3" t="s">
         <v>241</v>
       </c>
       <c r="K3">
-        <f>COUNTIF($A:$A,J3&amp;"*")</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="M3" t="s">
         <v>241</v>
       </c>
       <c r="N3">
-        <f>COUNTIF($A:$A,"*" &amp;M3)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
@@ -1431,22 +2421,22 @@
         <v>242</v>
       </c>
       <c r="H4">
-        <f>COUNTIF($A:$A,"*" &amp; G4&amp;"*")</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>27</v>
       </c>
       <c r="J4" t="s">
         <v>242</v>
       </c>
       <c r="K4">
-        <f>COUNTIF($A:$A,J4&amp;"*")</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="M4" t="s">
         <v>242</v>
       </c>
       <c r="N4">
-        <f>COUNTIF($A:$A,"*" &amp;M4)</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -1460,22 +2450,22 @@
         <v>243</v>
       </c>
       <c r="H5">
-        <f>COUNTIF($A:$A,"*" &amp; G5&amp;"*")</f>
-        <v>27</v>
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
       <c r="J5" t="s">
         <v>243</v>
       </c>
       <c r="K5">
-        <f>COUNTIF($A:$A,J5&amp;"*")</f>
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="M5" t="s">
         <v>243</v>
       </c>
       <c r="N5">
-        <f>COUNTIF($A:$A,"*" &amp;M5)</f>
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -1489,22 +2479,22 @@
         <v>244</v>
       </c>
       <c r="H6">
-        <f>COUNTIF($A:$A,"*" &amp; G6&amp;"*")</f>
-        <v>26</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J6" t="s">
         <v>244</v>
       </c>
       <c r="K6">
-        <f>COUNTIF($A:$A,J6&amp;"*")</f>
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="M6" t="s">
         <v>244</v>
       </c>
       <c r="N6">
-        <f>COUNTIF($A:$A,"*" &amp;M6)</f>
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -1518,22 +2508,22 @@
         <v>245</v>
       </c>
       <c r="H7">
-        <f>COUNTIF($A:$A,"*" &amp; G7&amp;"*")</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="J7" t="s">
         <v>245</v>
       </c>
       <c r="K7">
-        <f>COUNTIF($A:$A,J7&amp;"*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M7" t="s">
         <v>245</v>
       </c>
       <c r="N7">
-        <f>COUNTIF($A:$A,"*" &amp;M7)</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -1547,22 +2537,22 @@
         <v>246</v>
       </c>
       <c r="H8">
-        <f>COUNTIF($A:$A,"*" &amp; G8&amp;"*")</f>
-        <v>22</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="J8" t="s">
         <v>246</v>
       </c>
       <c r="K8">
-        <f>COUNTIF($A:$A,J8&amp;"*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M8" t="s">
         <v>246</v>
       </c>
       <c r="N8">
-        <f>COUNTIF($A:$A,"*" &amp;M8)</f>
-        <v>17</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -1576,21 +2566,21 @@
         <v>247</v>
       </c>
       <c r="H9">
-        <f>COUNTIF($A:$A,"*" &amp; G9&amp;"*")</f>
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J9" t="s">
         <v>247</v>
       </c>
       <c r="K9">
-        <f>COUNTIF($A:$A,J9&amp;"*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M9" t="s">
         <v>247</v>
       </c>
       <c r="N9">
-        <f>COUNTIF($A:$A,"*" &amp;M9)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1605,22 +2595,22 @@
         <v>248</v>
       </c>
       <c r="H10">
-        <f>COUNTIF($A:$A,"*" &amp; G10&amp;"*")</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>29</v>
       </c>
       <c r="J10" t="s">
         <v>248</v>
       </c>
       <c r="K10">
-        <f>COUNTIF($A:$A,J10&amp;"*")</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="M10" t="s">
         <v>248</v>
       </c>
       <c r="N10">
-        <f>COUNTIF($A:$A,"*" &amp;M10)</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -1634,22 +2624,22 @@
         <v>249</v>
       </c>
       <c r="H11">
-        <f>COUNTIF($A:$A,"*" &amp; G11&amp;"*")</f>
-        <v>29</v>
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
       <c r="J11" t="s">
         <v>249</v>
       </c>
       <c r="K11">
-        <f>COUNTIF($A:$A,J11&amp;"*")</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="M11" t="s">
         <v>249</v>
       </c>
       <c r="N11">
-        <f>COUNTIF($A:$A,"*" &amp;M11)</f>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -1663,22 +2653,22 @@
         <v>250</v>
       </c>
       <c r="H12">
-        <f>COUNTIF($A:$A,"*" &amp; G12&amp;"*")</f>
-        <v>26</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="J12" t="s">
         <v>250</v>
       </c>
       <c r="K12">
-        <f>COUNTIF($A:$A,J12&amp;"*")</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="M12" t="s">
         <v>250</v>
       </c>
       <c r="N12">
-        <f>COUNTIF($A:$A,"*" &amp;M12)</f>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -1692,21 +2682,21 @@
         <v>251</v>
       </c>
       <c r="H13">
-        <f>COUNTIF($A:$A,"*" &amp; G13&amp;"*")</f>
-        <v>19</v>
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="J13" t="s">
         <v>251</v>
       </c>
       <c r="K13">
-        <f>COUNTIF($A:$A,J13&amp;"*")</f>
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="M13" t="s">
         <v>251</v>
       </c>
       <c r="N13">
-        <f>COUNTIF($A:$A,"*" &amp;M13)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1721,22 +2711,22 @@
         <v>252</v>
       </c>
       <c r="H14">
-        <f>COUNTIF($A:$A,"*" &amp; G14&amp;"*")</f>
-        <v>24</v>
+        <f t="shared" si="0"/>
+        <v>36</v>
       </c>
       <c r="J14" t="s">
         <v>252</v>
       </c>
       <c r="K14">
-        <f>COUNTIF($A:$A,J14&amp;"*")</f>
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>17</v>
       </c>
       <c r="M14" t="s">
         <v>252</v>
       </c>
       <c r="N14">
-        <f>COUNTIF($A:$A,"*" &amp;M14)</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1750,22 +2740,22 @@
         <v>253</v>
       </c>
       <c r="H15">
-        <f>COUNTIF($A:$A,"*" &amp; G15&amp;"*")</f>
-        <v>36</v>
+        <f t="shared" si="0"/>
+        <v>37</v>
       </c>
       <c r="J15" t="s">
         <v>253</v>
       </c>
       <c r="K15">
-        <f>COUNTIF($A:$A,J15&amp;"*")</f>
-        <v>17</v>
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="M15" t="s">
         <v>253</v>
       </c>
       <c r="N15">
-        <f>COUNTIF($A:$A,"*" &amp;M15)</f>
-        <v>11</v>
+        <f t="shared" si="2"/>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1779,21 +2769,21 @@
         <v>254</v>
       </c>
       <c r="H16">
-        <f>COUNTIF($A:$A,"*" &amp; G16&amp;"*")</f>
-        <v>37</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="J16" t="s">
         <v>254</v>
       </c>
       <c r="K16">
-        <f>COUNTIF($A:$A,J16&amp;"*")</f>
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="M16" t="s">
         <v>254</v>
       </c>
       <c r="N16">
-        <f>COUNTIF($A:$A,"*" &amp;M16)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
     </row>
@@ -1808,22 +2798,22 @@
         <v>255</v>
       </c>
       <c r="H17">
-        <f>COUNTIF($A:$A,"*" &amp; G17&amp;"*")</f>
-        <v>18</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="J17" t="s">
         <v>255</v>
       </c>
       <c r="K17">
-        <f>COUNTIF($A:$A,J17&amp;"*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M17" t="s">
         <v>255</v>
       </c>
       <c r="N17">
-        <f>COUNTIF($A:$A,"*" &amp;M17)</f>
-        <v>13</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -1833,27 +2823,6 @@
       <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="G18" t="s">
-        <v>256</v>
-      </c>
-      <c r="H18">
-        <f>COUNTIF($A:$A,"*" &amp; G18&amp;"*")</f>
-        <v>3</v>
-      </c>
-      <c r="J18" t="s">
-        <v>256</v>
-      </c>
-      <c r="K18">
-        <f>COUNTIF($A:$A,J18&amp;"*")</f>
-        <v>0</v>
-      </c>
-      <c r="M18" t="s">
-        <v>256</v>
-      </c>
-      <c r="N18">
-        <f>COUNTIF($A:$A,"*" &amp;M18)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -1862,13 +2831,6 @@
       <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="G19" t="s">
-        <v>257</v>
-      </c>
-      <c r="H19">
-        <f>COUNTIF($A:$A,"*" &amp; G19&amp;"*")</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -1877,13 +2839,6 @@
       <c r="B20" t="s">
         <v>39</v>
       </c>
-      <c r="G20" t="s">
-        <v>258</v>
-      </c>
-      <c r="H20">
-        <f>COUNTIF($A:$A,"*" &amp; G20&amp;"*")</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -2538,7 +3493,7 @@
         <v>202</v>
       </c>
       <c r="B102" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
@@ -2693,260 +3648,1595 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B6" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C6" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B8" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B9" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C9" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B10" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C10" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C11" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B12" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B13" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C13" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B14" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B15" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C15" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B16" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C16" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B17" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B18" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B19" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B20" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B21" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B22" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B23" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B24" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>322</v>
+      </c>
+      <c r="B25" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>325</v>
       </c>
+      <c r="B28" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>329</v>
+      </c>
+      <c r="B32" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>330</v>
+      </c>
+      <c r="B33" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>331</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>334</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>259</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>337</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>355</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>357</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>359</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>361</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>363</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>365</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>367</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>369</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>371</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>352</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>373</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>287</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>375</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>377</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>379</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>381</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>291</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>384</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>275</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>386</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>388</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>390</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>392</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>343</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>316</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>394</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>396</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>398</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>400</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>402</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>404</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>406</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>408</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>410</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>412</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>389</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>395</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>414</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>416</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>319</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>354</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>418</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>420</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>422</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>426</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>428</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>430</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>432</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>434</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>435</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>437</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>439</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>441</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>443</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>445</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>447</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>449</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>451</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>453</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>455</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>457</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>459</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>461</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>463</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>465</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>467</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>468</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B1" t="s">
+        <v>645</v>
+      </c>
+      <c r="C1" t="s">
+        <v>648</v>
+      </c>
+      <c r="G1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>469</v>
+      </c>
+      <c r="B2" t="s">
+        <v>470</v>
+      </c>
+      <c r="C2" t="s">
+        <v>471</v>
+      </c>
+      <c r="G2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B3" t="s">
+        <v>474</v>
+      </c>
+      <c r="C3" t="s">
+        <v>475</v>
+      </c>
+      <c r="G3" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>477</v>
+      </c>
+      <c r="B4" t="s">
+        <v>478</v>
+      </c>
+      <c r="C4" t="s">
+        <v>479</v>
+      </c>
+      <c r="G4" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>481</v>
+      </c>
+      <c r="B5" t="s">
+        <v>482</v>
+      </c>
+      <c r="C5" t="s">
+        <v>483</v>
+      </c>
+      <c r="G5" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>485</v>
+      </c>
+      <c r="B6" t="s">
+        <v>486</v>
+      </c>
+      <c r="C6" t="s">
+        <v>487</v>
+      </c>
+      <c r="G6" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>489</v>
+      </c>
+      <c r="B7" t="s">
+        <v>490</v>
+      </c>
+      <c r="C7" t="s">
+        <v>491</v>
+      </c>
+      <c r="G7" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>493</v>
+      </c>
+      <c r="B8" t="s">
+        <v>494</v>
+      </c>
+      <c r="C8" t="s">
+        <v>495</v>
+      </c>
+      <c r="G8" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>497</v>
+      </c>
+      <c r="B9" t="s">
+        <v>498</v>
+      </c>
+      <c r="C9" t="s">
+        <v>499</v>
+      </c>
+      <c r="G9" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>501</v>
+      </c>
+      <c r="B10" t="s">
+        <v>502</v>
+      </c>
+      <c r="C10" t="s">
+        <v>503</v>
+      </c>
+      <c r="G10" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>505</v>
+      </c>
+      <c r="B11" t="s">
+        <v>506</v>
+      </c>
+      <c r="C11" t="s">
+        <v>507</v>
+      </c>
+      <c r="G11" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>509</v>
+      </c>
+      <c r="B12" t="s">
+        <v>510</v>
+      </c>
+      <c r="C12" t="s">
+        <v>511</v>
+      </c>
+      <c r="G12" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>513</v>
+      </c>
+      <c r="B13" t="s">
+        <v>514</v>
+      </c>
+      <c r="C13" t="s">
+        <v>515</v>
+      </c>
+      <c r="G13" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>517</v>
+      </c>
+      <c r="B14" t="s">
+        <v>518</v>
+      </c>
+      <c r="C14" t="s">
+        <v>519</v>
+      </c>
+      <c r="G14" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>521</v>
+      </c>
+      <c r="B15" t="s">
+        <v>522</v>
+      </c>
+      <c r="C15" t="s">
+        <v>523</v>
+      </c>
+      <c r="G15" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>525</v>
+      </c>
+      <c r="B16" t="s">
+        <v>526</v>
+      </c>
+      <c r="C16" t="s">
+        <v>527</v>
+      </c>
+      <c r="G16" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>529</v>
+      </c>
+      <c r="B17" t="s">
+        <v>530</v>
+      </c>
+      <c r="C17" t="s">
+        <v>531</v>
+      </c>
+      <c r="G17" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>533</v>
+      </c>
+      <c r="B18" t="s">
+        <v>534</v>
+      </c>
+      <c r="C18" t="s">
+        <v>535</v>
+      </c>
+      <c r="G18" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>537</v>
+      </c>
+      <c r="B19" t="s">
+        <v>538</v>
+      </c>
+      <c r="C19" t="s">
+        <v>539</v>
+      </c>
+      <c r="G19" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>541</v>
+      </c>
+      <c r="B20" t="s">
+        <v>542</v>
+      </c>
+      <c r="C20" t="s">
+        <v>543</v>
+      </c>
+      <c r="G20" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>545</v>
+      </c>
+      <c r="B21" t="s">
+        <v>546</v>
+      </c>
+      <c r="C21" t="s">
+        <v>547</v>
+      </c>
+      <c r="G21" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>549</v>
+      </c>
+      <c r="B22" t="s">
+        <v>550</v>
+      </c>
+      <c r="C22" t="s">
+        <v>551</v>
+      </c>
+      <c r="G22" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>553</v>
+      </c>
+      <c r="B23" t="s">
+        <v>554</v>
+      </c>
+      <c r="C23" t="s">
+        <v>555</v>
+      </c>
+      <c r="G23" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>557</v>
+      </c>
+      <c r="B24" t="s">
+        <v>558</v>
+      </c>
+      <c r="C24" t="s">
+        <v>559</v>
+      </c>
+      <c r="G24" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>561</v>
+      </c>
       <c r="B25" t="s">
-        <v>324</v>
+        <v>562</v>
+      </c>
+      <c r="C25" t="s">
+        <v>563</v>
+      </c>
+      <c r="G25" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>565</v>
+      </c>
+      <c r="B26" t="s">
+        <v>566</v>
+      </c>
+      <c r="C26" t="s">
+        <v>567</v>
+      </c>
+      <c r="G26" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>569</v>
+      </c>
+      <c r="B27" t="s">
+        <v>570</v>
+      </c>
+      <c r="C27" t="s">
+        <v>571</v>
+      </c>
+      <c r="G27" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>573</v>
+      </c>
+      <c r="B28" t="s">
+        <v>574</v>
+      </c>
+      <c r="C28" t="s">
+        <v>575</v>
+      </c>
+      <c r="G28" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>577</v>
+      </c>
+      <c r="B29" t="s">
+        <v>578</v>
+      </c>
+      <c r="C29" t="s">
+        <v>579</v>
+      </c>
+      <c r="G29" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>581</v>
+      </c>
+      <c r="B30" t="s">
+        <v>582</v>
+      </c>
+      <c r="C30" t="s">
+        <v>583</v>
+      </c>
+      <c r="G30" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>585</v>
+      </c>
+      <c r="B31" t="s">
+        <v>586</v>
+      </c>
+      <c r="C31" t="s">
+        <v>587</v>
+      </c>
+      <c r="G31" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>589</v>
+      </c>
+      <c r="B32" t="s">
+        <v>590</v>
+      </c>
+      <c r="C32" t="s">
+        <v>591</v>
+      </c>
+      <c r="G32" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>593</v>
+      </c>
+      <c r="B33" t="s">
+        <v>594</v>
+      </c>
+      <c r="C33" t="s">
+        <v>595</v>
+      </c>
+      <c r="G33" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>597</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="C34" t="s">
+        <v>599</v>
+      </c>
+      <c r="G34" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>601</v>
+      </c>
+      <c r="B35" t="s">
+        <v>602</v>
+      </c>
+      <c r="C35" t="s">
+        <v>603</v>
+      </c>
+      <c r="G35" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>605</v>
+      </c>
+      <c r="B36" t="s">
+        <v>606</v>
+      </c>
+      <c r="C36" t="s">
+        <v>607</v>
+      </c>
+      <c r="G36" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>609</v>
+      </c>
+      <c r="B37" t="s">
+        <v>610</v>
+      </c>
+      <c r="C37" t="s">
+        <v>611</v>
+      </c>
+      <c r="G37" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>613</v>
+      </c>
+      <c r="B38" t="s">
+        <v>614</v>
+      </c>
+      <c r="C38" t="s">
+        <v>615</v>
+      </c>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>616</v>
+      </c>
+      <c r="B39" t="s">
+        <v>617</v>
+      </c>
+      <c r="C39" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>619</v>
+      </c>
+      <c r="B40" t="s">
+        <v>620</v>
+      </c>
+      <c r="C40" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>622</v>
+      </c>
+      <c r="B41" t="s">
+        <v>623</v>
+      </c>
+      <c r="C41" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>625</v>
+      </c>
+      <c r="B42" t="s">
+        <v>626</v>
+      </c>
+      <c r="C42" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>628</v>
+      </c>
+      <c r="B43" t="s">
+        <v>629</v>
+      </c>
+      <c r="C43" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>631</v>
+      </c>
+      <c r="B44" t="s">
+        <v>632</v>
+      </c>
+      <c r="C44" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>634</v>
+      </c>
+      <c r="B45" t="s">
+        <v>635</v>
+      </c>
+      <c r="C45" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>637</v>
+      </c>
+      <c r="B46" t="s">
+        <v>371</v>
+      </c>
+      <c r="C46" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>639</v>
+      </c>
+      <c r="B47" t="s">
+        <v>640</v>
+      </c>
+      <c r="C47" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>642</v>
+      </c>
+      <c r="B48" t="s">
+        <v>643</v>
+      </c>
+      <c r="C48" t="s">
+        <v>644</v>
       </c>
     </row>
   </sheetData>

</xml_diff>